<commit_message>
Adicionar e remover comodo
</commit_message>
<xml_diff>
--- a/Casa_comodos.xlsx
+++ b/Casa_comodos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,10 +436,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Joao</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Breno</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>